<commit_message>
allowsplits is now false by default
</commit_message>
<xml_diff>
--- a/doc/examples/buffer/transfer-batch.xlsx
+++ b/doc/examples/buffer/transfer-batch.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\user-guide\cookbook\buffer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\community-u20\doc\examples\buffer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ADB950-7F10-45ED-8A46-F3ED812FE849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22823" windowHeight="7380" tabRatio="763" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="2688" yWindow="1776" windowWidth="17232" windowHeight="11184" tabRatio="763" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -307,12 +308,18 @@
   </si>
   <si>
     <t>2. make subassembly</t>
+  </si>
+  <si>
+    <t>allowsplits</t>
+  </si>
+  <si>
+    <t>Controls whether a sales order or forecast can be split across multiple manufacturing orders during planning. Default: false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
@@ -361,7 +368,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="headerstyle" xfId="1"/>
+    <cellStyle name="headerstyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,23 +668,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -759,26 +766,26 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1048576"/>
+  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.19921875" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -882,26 +889,26 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1048576"/>
+  <autoFilter ref="A1:F1048576" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1052,22 +1059,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048576"/>
+  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1127,24 +1134,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1048576"/>
+  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="136.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1257,23 +1264,34 @@
         <v>84</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C1048521"/>
+  <autoFilter ref="A1:C1048521" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1312,20 +1330,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048575"/>
+  <autoFilter ref="A1:A1048575" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -1353,20 +1371,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1048575"/>
+  <autoFilter ref="A1:B1048575" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -1379,20 +1397,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -1468,22 +1486,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1048576"/>
+  <autoFilter ref="A1:D1048576" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1502,23 +1520,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048568"/>
+  <autoFilter ref="A1:A1048568" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1573,20 +1591,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048576"/>
+  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1602,23 +1620,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048575"/>
+  <autoFilter ref="A1:A1048575" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1710,7 +1728,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1048575"/>
+  <autoFilter ref="A1:N1048575" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>